<commit_message>
1. go on renesas
</commit_message>
<xml_diff>
--- a/TRenesasAll_105H/bom_price.xlsx
+++ b/TRenesasAll_105H/bom_price.xlsx
@@ -1,45 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuhe/Desktop/TaskModel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BB55D9-23F6-C047-AC9F-739372BDC2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="bom_price" sheetId="2" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bom_price" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <family val="3"/>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -58,21 +53,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -360,14 +414,170 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D707305E-F1CE-1A43-A0C4-768AD7A067F3}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>71V67603S166PFGI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Renesas</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>《此供应商选择了隐藏公司名》</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>￥19</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>两年前</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>&lt;50</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-05-05</t>
+        </is>
+      </c>
+      <c r="J1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>71V67603S166PFGI</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Renesas</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>《此供应商选择了隐藏公司名》</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>￥19</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>两年前</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>&lt;50</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-05-05</t>
+        </is>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>71V67603S166PFGI</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Renesas</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>《此供应商选择了隐藏公司名》</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>**</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>￥19</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>两年前</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>&lt;50</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-05-05</t>
+        </is>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>